<commit_message>
Add latest analysis / proposal for UKWA
</commit_message>
<xml_diff>
--- a/resources/ukwa/analysis/participants.xlsx
+++ b/resources/ukwa/analysis/participants.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wsw-results\resources\ukwa\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E4777-12EB-4CE3-8483-30968CA8AA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE4A48-FA9A-4F16-9917-ED2C69AE3842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Pro</t>
   </si>
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -124,7 +124,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -159,6 +159,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Percentages in each fleet</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -221,84 +246,102 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:f>Sheet1!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,84 +378,102 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$13</c:f>
+              <c:f>Sheet1!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,84 +510,102 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$13</c:f>
+              <c:f>Sheet1!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="13">
                   <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,7 +1670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
@@ -1646,35 +1725,35 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2023</v>
+        <v>2010</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <f>SUM(B3:D3)</f>
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="G3">
-        <v>2023</v>
+        <v>2010</v>
       </c>
       <c r="H3" s="4">
         <f>B3/$E3</f>
-        <v>0.16666666666666666</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I3" s="4">
         <f>C3/$E3</f>
-        <v>0.40740740740740738</v>
+        <v>0.34343434343434343</v>
       </c>
       <c r="J3" s="4">
         <f>D3/$E3</f>
-        <v>0.42592592592592593</v>
+        <v>0.56565656565656564</v>
       </c>
       <c r="L3" s="1">
         <v>4</v>
@@ -1682,35 +1761,35 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="B4" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E13" si="0">SUM(B4:D4)</f>
-        <v>63</v>
+        <f>SUM(B4:D4)</f>
+        <v>88</v>
       </c>
       <c r="G4">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="H4" s="4">
         <f>B4/$E4</f>
-        <v>0.22222222222222221</v>
+        <v>0.14772727272727273</v>
       </c>
       <c r="I4" s="4">
         <f>C4/$E4</f>
-        <v>0.38095238095238093</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="J4" s="4">
         <f>D4/$E4</f>
-        <v>0.3968253968253968</v>
+        <v>0.48863636363636365</v>
       </c>
       <c r="L4" s="1">
         <v>9</v>
@@ -1718,35 +1797,35 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>SUM(B5:D5)</f>
+        <v>80</v>
       </c>
       <c r="G5">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="H5" s="4">
         <f>B5/$E5</f>
-        <v>0.29411764705882354</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="I5" s="4">
         <f>C5/$E5</f>
-        <v>0.41176470588235292</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="J5" s="4">
         <f>D5/$E5</f>
-        <v>0.29411764705882354</v>
+        <v>0.5</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
@@ -1757,32 +1836,35 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2020</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>2013</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUM(B6:D6)</f>
+        <v>63</v>
+      </c>
       <c r="G6">
-        <v>2020</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>4</v>
+        <v>2013</v>
+      </c>
+      <c r="H6" s="4">
+        <f>B6/$E6</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="I6" s="4">
+        <f>C6/$E6</f>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="J6" s="4">
+        <f>D6/$E6</f>
+        <v>0.41269841269841268</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1791,35 +1873,35 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B7" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>19</v>
       </c>
       <c r="D7" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>SUM(B7:D7)</f>
+        <v>61</v>
       </c>
       <c r="G7">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="H7" s="4">
         <f>B7/$E7</f>
-        <v>0.20754716981132076</v>
+        <v>0.14754098360655737</v>
       </c>
       <c r="I7" s="4">
         <f>C7/$E7</f>
-        <v>0.35849056603773582</v>
+        <v>0.31147540983606559</v>
       </c>
       <c r="J7" s="4">
         <f>D7/$E7</f>
-        <v>0.43396226415094341</v>
+        <v>0.54098360655737709</v>
       </c>
       <c r="L7" s="1">
         <v>5</v>
@@ -1827,35 +1909,35 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="B8" s="1">
         <v>12</v>
       </c>
       <c r="C8" s="1">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <f>SUM(B8:D8)</f>
+        <v>64</v>
       </c>
       <c r="G8">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="H8" s="4">
         <f>B8/$E8</f>
-        <v>0.20689655172413793</v>
+        <v>0.1875</v>
       </c>
       <c r="I8" s="4">
         <f>C8/$E8</f>
-        <v>0.32758620689655171</v>
+        <v>0.46875</v>
       </c>
       <c r="J8" s="4">
         <f>D8/$E8</f>
-        <v>0.46551724137931033</v>
+        <v>0.34375</v>
       </c>
       <c r="L8" s="1">
         <v>8</v>
@@ -1863,35 +1945,35 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B9" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <f>SUM(B9:D9)</f>
+        <v>68</v>
       </c>
       <c r="G9">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="H9" s="4">
         <f>B9/$E9</f>
-        <v>0.25925925925925924</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="I9" s="4">
         <f>C9/$E9</f>
-        <v>0.29629629629629628</v>
+        <v>0.36764705882352944</v>
       </c>
       <c r="J9" s="4">
         <f>D9/$E9</f>
-        <v>0.44444444444444442</v>
+        <v>0.45588235294117646</v>
       </c>
       <c r="L9" s="1">
         <v>6</v>
@@ -1899,35 +1981,35 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B10" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>SUM(B10:D10)</f>
+        <v>54</v>
       </c>
       <c r="G10">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="H10" s="4">
         <f>B10/$E10</f>
-        <v>0.17647058823529413</v>
+        <v>0.25925925925925924</v>
       </c>
       <c r="I10" s="4">
         <f>C10/$E10</f>
-        <v>0.36764705882352944</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="J10" s="4">
         <f>D10/$E10</f>
-        <v>0.45588235294117646</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L10" s="1">
         <v>7</v>
@@ -1935,35 +2017,35 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B11" s="1">
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <f>SUM(B11:D11)</f>
+        <v>58</v>
       </c>
       <c r="G11">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="H11" s="4">
         <f>B11/$E11</f>
-        <v>0.1875</v>
+        <v>0.20689655172413793</v>
       </c>
       <c r="I11" s="4">
         <f>C11/$E11</f>
-        <v>0.46875</v>
+        <v>0.32758620689655171</v>
       </c>
       <c r="J11" s="4">
         <f>D11/$E11</f>
-        <v>0.34375</v>
+        <v>0.46551724137931033</v>
       </c>
       <c r="L11" s="1">
         <v>5</v>
@@ -1971,35 +2053,35 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>19</v>
       </c>
       <c r="D12" s="1">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <f>SUM(B12:D12)</f>
+        <v>53</v>
       </c>
       <c r="G12">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="H12" s="4">
         <f>B12/$E12</f>
-        <v>0.14754098360655737</v>
+        <v>0.20754716981132076</v>
       </c>
       <c r="I12" s="4">
         <f>C12/$E12</f>
-        <v>0.31147540983606559</v>
+        <v>0.35849056603773582</v>
       </c>
       <c r="J12" s="4">
         <f>D12/$E12</f>
-        <v>0.54098360655737709</v>
+        <v>0.43396226415094341</v>
       </c>
       <c r="L12" s="1">
         <v>7</v>
@@ -2007,69 +2089,180 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2013</v>
-      </c>
-      <c r="B13" s="1">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1">
-        <v>26</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
+        <v>2020</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="G13">
-        <v>2013</v>
-      </c>
-      <c r="H13" s="4">
-        <f>B13/$E13</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="I13" s="4">
-        <f>C13/$E13</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="J13" s="4">
-        <f>D13/$E13</f>
-        <v>0.41269841269841268</v>
+        <v>2020</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2021</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUM(B14:D14)</f>
+        <v>17</v>
+      </c>
+      <c r="G14">
+        <v>2021</v>
+      </c>
+      <c r="H14" s="4">
+        <f>B14/$E14</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="I14" s="4">
+        <f>C14/$E14</f>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="J14" s="4">
+        <f>D14/$E14</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="5">
-        <f>AVERAGE(L3:L13)</f>
-        <v>6.1111111111111107</v>
+      <c r="A15">
+        <v>2022</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUM(B15:D15)</f>
+        <v>63</v>
+      </c>
+      <c r="G15">
+        <v>2022</v>
+      </c>
+      <c r="H15" s="4">
+        <f>B15/$E15</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="I15" s="4">
+        <f>C15/$E15</f>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="J15" s="4">
+        <f>D15/$E15</f>
+        <v>0.3968253968253968</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K16" s="1" t="s">
+      <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUM(B16:D16)</f>
+        <v>54</v>
+      </c>
+      <c r="G16">
+        <v>2023</v>
+      </c>
+      <c r="H16" s="4">
+        <f>B16/$E16</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I16" s="4">
+        <f>C16/$E16</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J16" s="4">
+        <f>D16/$E16</f>
+        <v>0.42592592592592593</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="5">
+        <f>AVERAGE(L3:L19)</f>
+        <v>6.1111111111111107</v>
+      </c>
+    </row>
+    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="5">
-        <f>MEDIAN(L3:L13)</f>
+      <c r="L21" s="5">
+        <f>MEDIAN(L3:L19)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K18" s="1" t="s">
+    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="4">
-        <f>0.25*L3/L16</f>
+      <c r="L23" s="4">
+        <f>0.25*L3/L21</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J16">
+    <sortCondition ref="A3:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E3:E16" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>